<commit_message>
checking pipeline run 02
</commit_message>
<xml_diff>
--- a/heartbeat base xlsx template_copy(2).xlsx
+++ b/heartbeat base xlsx template_copy(2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://docs.philips.com/personal/ananyak_s_philips_com/Documents/Saved Pictures/VS Files/heartbeat generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_496DC3F704648CFEE77960B543245E3FB48F8EF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0C18250-3806-4AED-B9A1-6EC96EC7DE57}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_496DC3F704648CFEE77960B543245E3FB48F8EF1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F939C56-A99C-4CB2-8598-E2A6CEF107D5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,7 +154,7 @@
     <t>1s</t>
   </si>
   <si>
-    <t>site</t>
+    <t>hello</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>